<commit_message>
Correct elec/IiCFfNPdtTI so increases are relative to the first year, not the immediately preceeding year (#232)
</commit_message>
<xml_diff>
--- a/InputData/elec/IiCFfNPdtTI/Inc in Cap Factors due to Tech Imprv.xlsx
+++ b/InputData/elec/IiCFfNPdtTI/Inc in Cap Factors due to Tech Imprv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\IiCFfNPdtTI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\IiCFfNPdtTI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C59D57A-2D4F-4D92-A1F3-ADACA93CB5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9286D0BD-423E-48AD-9774-71EB3C4BD8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3A6AC5FA-76A9-4F78-AA3D-672D999FE94A}"/>
+    <workbookView xWindow="25185" yWindow="1770" windowWidth="28710" windowHeight="18495" xr2:uid="{3A6AC5FA-76A9-4F78-AA3D-672D999FE94A}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>About</t>
-  </si>
-  <si>
-    <t>This file should contain time-series multipliers reflecting the increase in capacity factor for newly built plants of each plant type</t>
   </si>
   <si>
     <t>(applied to all hours) due to technological advances in plant technology, such as solar PV panels capable of converting a higher percentage of</t>
@@ -501,6 +498,9 @@
   <si>
     <t>Solar and Wind</t>
   </si>
+  <si>
+    <t>This file should contain time-series multipliers reflecting the increase in capacity factor for newly built plants of each plant type relative to the Start Year</t>
+  </si>
 </sst>
 </file>
 
@@ -833,12 +833,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -909,7 +903,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -917,6 +910,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1235,13 +1235,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D9DCC6-C096-4365-BF94-479BB0461914}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1253,37 +1251,37 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="53" t="s">
-        <v>153</v>
+      <c r="B3" s="50" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="51" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="54" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="52" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="55" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="52" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="55" t="s">
-        <v>152</v>
-      </c>
-    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="55"/>
+      <c r="B9" s="52"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1292,42 +1290,42 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1343,9 +1341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19171EFF-FEE2-41E4-9EC7-9C84E5EE47DC}">
   <dimension ref="A1:BJ154"/>
   <sheetViews>
-    <sheetView topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="G146" sqref="G146"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1355,7 +1351,7 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1393,7 +1389,7 @@
     </row>
     <row r="2" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1494,7 +1490,7 @@
     </row>
     <row r="4" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6">
@@ -1593,7 +1589,7 @@
     </row>
     <row r="5" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8">
@@ -1692,7 +1688,7 @@
     </row>
     <row r="6" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10">
@@ -1791,7 +1787,7 @@
     </row>
     <row r="7" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6">
@@ -1890,7 +1886,7 @@
     </row>
     <row r="8" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8">
@@ -1989,7 +1985,7 @@
     </row>
     <row r="9" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10">
@@ -2088,7 +2084,7 @@
     </row>
     <row r="10" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6">
@@ -2187,7 +2183,7 @@
     </row>
     <row r="11" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8">
@@ -2286,7 +2282,7 @@
     </row>
     <row r="12" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10">
@@ -2385,7 +2381,7 @@
     </row>
     <row r="13" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6">
@@ -2484,7 +2480,7 @@
     </row>
     <row r="14" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8">
@@ -2583,7 +2579,7 @@
     </row>
     <row r="15" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10">
@@ -2682,7 +2678,7 @@
     </row>
     <row r="16" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6">
@@ -2781,7 +2777,7 @@
     </row>
     <row r="17" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8">
@@ -2880,7 +2876,7 @@
     </row>
     <row r="18" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10">
@@ -2979,7 +2975,7 @@
     </row>
     <row r="19" spans="1:34" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19">
         <v>0.24546183884659542</v>
@@ -3078,7 +3074,7 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20">
         <v>0.24368540488531945</v>
@@ -3177,7 +3173,7 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21">
         <v>0.24108344017238761</v>
@@ -3276,7 +3272,7 @@
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22">
         <v>0.26274189125582154</v>
@@ -3375,7 +3371,7 @@
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23">
         <v>0.26084039968030859</v>
@@ -3474,7 +3470,7 @@
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24">
         <v>0.25805526153879943</v>
@@ -3573,7 +3569,7 @@
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25">
         <v>0.27801629364985952</v>
@@ -3671,7 +3667,7 @@
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26">
         <v>0.27600425956689018</v>
@@ -3769,7 +3765,7 @@
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27">
         <v>0.27305720845256554</v>
@@ -3867,7 +3863,7 @@
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28">
         <v>0.29150681399764794</v>
@@ -3965,7 +3961,7 @@
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29">
         <v>0.28939714755514884</v>
@@ -4063,7 +4059,7 @@
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30">
         <v>0.28630709312076041</v>
@@ -4161,7 +4157,7 @@
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31">
         <v>0.3005277955541486</v>
@@ -4259,7 +4255,7 @@
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32">
         <v>0.29835284328931427</v>
@@ -4357,7 +4353,7 @@
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33">
         <v>0.29516716390647635</v>
@@ -4455,7 +4451,7 @@
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="11">
@@ -4586,7 +4582,7 @@
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -4720,7 +4716,7 @@
     </row>
     <row r="40" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6">
@@ -4819,7 +4815,7 @@
     </row>
     <row r="41" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8">
@@ -4918,7 +4914,7 @@
     </row>
     <row r="42" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10">
@@ -5017,7 +5013,7 @@
     </row>
     <row r="43" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6">
@@ -5116,7 +5112,7 @@
     </row>
     <row r="44" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8">
@@ -5215,7 +5211,7 @@
     </row>
     <row r="45" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10">
@@ -5314,7 +5310,7 @@
     </row>
     <row r="46" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="6">
@@ -5413,7 +5409,7 @@
     </row>
     <row r="47" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8">
@@ -5512,7 +5508,7 @@
     </row>
     <row r="48" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="10">
@@ -5614,7 +5610,7 @@
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50" s="13">
         <f>AVERAGE(C41,C44,C47)</f>
@@ -5747,7 +5743,7 @@
     </row>
     <row r="52" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -5881,7 +5877,7 @@
     </row>
     <row r="54" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B54" s="15"/>
       <c r="C54" s="15">
@@ -5980,7 +5976,7 @@
     </row>
     <row r="55" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B55" s="16"/>
       <c r="C55" s="16">
@@ -6079,7 +6075,7 @@
     </row>
     <row r="56" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B56" s="18"/>
       <c r="C56" s="18">
@@ -6178,7 +6174,7 @@
     </row>
     <row r="57" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B57" s="15"/>
       <c r="C57" s="15">
@@ -6277,7 +6273,7 @@
     </row>
     <row r="58" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B58" s="16"/>
       <c r="C58" s="16">
@@ -6376,7 +6372,7 @@
     </row>
     <row r="59" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B59" s="18"/>
       <c r="C59" s="18">
@@ -6475,7 +6471,7 @@
     </row>
     <row r="60" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B60" s="15"/>
       <c r="C60" s="15">
@@ -6574,7 +6570,7 @@
     </row>
     <row r="61" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B61" s="16"/>
       <c r="C61" s="16">
@@ -6673,7 +6669,7 @@
     </row>
     <row r="62" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B62" s="19"/>
       <c r="C62" s="19">
@@ -6772,7 +6768,7 @@
     </row>
     <row r="63" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B63" s="15"/>
       <c r="C63" s="15">
@@ -6871,7 +6867,7 @@
     </row>
     <row r="64" spans="1:34" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B64" s="16"/>
       <c r="C64" s="16">
@@ -6970,7 +6966,7 @@
     </row>
     <row r="65" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B65" s="19"/>
       <c r="C65" s="19">
@@ -7069,7 +7065,7 @@
     </row>
     <row r="66" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B66" s="15"/>
       <c r="C66" s="15">
@@ -7168,7 +7164,7 @@
     </row>
     <row r="67" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B67" s="16"/>
       <c r="C67" s="16">
@@ -7267,7 +7263,7 @@
     </row>
     <row r="68" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B68" s="19"/>
       <c r="C68" s="19">
@@ -7366,7 +7362,7 @@
     </row>
     <row r="69" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A69" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B69" s="15"/>
       <c r="C69" s="15">
@@ -7465,7 +7461,7 @@
     </row>
     <row r="70" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B70" s="16"/>
       <c r="C70" s="16">
@@ -7564,7 +7560,7 @@
     </row>
     <row r="71" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B71" s="19"/>
       <c r="C71" s="19">
@@ -7663,7 +7659,7 @@
     </row>
     <row r="72" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A72" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B72" s="15"/>
       <c r="C72" s="15">
@@ -7762,7 +7758,7 @@
     </row>
     <row r="73" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B73" s="16"/>
       <c r="C73" s="16">
@@ -7861,7 +7857,7 @@
     </row>
     <row r="74" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B74" s="19"/>
       <c r="C74" s="19">
@@ -7960,7 +7956,7 @@
     </row>
     <row r="75" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B75" s="15"/>
       <c r="C75" s="15">
@@ -8059,7 +8055,7 @@
     </row>
     <row r="76" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B76" s="16"/>
       <c r="C76" s="16">
@@ -8158,7 +8154,7 @@
     </row>
     <row r="77" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B77" s="19"/>
       <c r="C77" s="19">
@@ -8257,7 +8253,7 @@
     </row>
     <row r="78" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A78" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B78" s="15"/>
       <c r="C78" s="15">
@@ -8356,7 +8352,7 @@
     </row>
     <row r="79" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B79" s="16"/>
       <c r="C79" s="16">
@@ -8473,7 +8469,7 @@
     </row>
     <row r="80" spans="1:62" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B80" s="18"/>
       <c r="C80" s="18">
@@ -8590,7 +8586,7 @@
     </row>
     <row r="81" spans="1:39" s="3" customFormat="1" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A81" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B81" s="15"/>
       <c r="C81" s="15">
@@ -8689,7 +8685,7 @@
     </row>
     <row r="82" spans="1:39" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B82" s="16"/>
       <c r="C82" s="16">
@@ -8788,7 +8784,7 @@
     </row>
     <row r="83" spans="1:39" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B83" s="16"/>
       <c r="C83" s="16">
@@ -8890,31 +8886,31 @@
     </row>
     <row r="85" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B85" s="23"/>
       <c r="C85" s="23"/>
       <c r="D85" s="23"/>
     </row>
     <row r="86" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A86" s="24" t="s">
+      <c r="A86" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="B86" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="B86" s="24" t="s">
+      <c r="C86" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="C86" s="24" t="s">
+      <c r="D86" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="D86" s="24" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="87" spans="1:39" ht="50.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="25"/>
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
+      <c r="A87" s="54"/>
+      <c r="B87" s="54"/>
+      <c r="C87" s="54"/>
+      <c r="D87" s="54"/>
       <c r="G87">
         <f>B53</f>
         <v>0</v>
@@ -9045,16 +9041,16 @@
       </c>
     </row>
     <row r="88" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A88" s="26" t="s">
+      <c r="A88" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B88" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="B88" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="C88" s="28">
+      <c r="C88" s="26">
         <v>9.5</v>
       </c>
-      <c r="D88" s="29">
+      <c r="D88" s="27">
         <v>153</v>
       </c>
       <c r="F88" s="13" t="str">
@@ -9192,16 +9188,16 @@
       <c r="AM88" s="13"/>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A89" s="30" t="s">
+      <c r="A89" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B89" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B89" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="C89" s="32">
+      <c r="C89" s="30">
         <v>8.9</v>
       </c>
-      <c r="D89" s="33">
+      <c r="D89" s="31">
         <v>152</v>
       </c>
       <c r="F89" s="13" t="str">
@@ -9339,16 +9335,16 @@
       <c r="AM89" s="13"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A90" s="34" t="s">
+      <c r="A90" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="B90" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="B90" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C90" s="36">
+      <c r="C90" s="34">
         <v>8.6999999999999993</v>
       </c>
-      <c r="D90" s="37">
+      <c r="D90" s="35">
         <v>304</v>
       </c>
       <c r="F90" s="13" t="str">
@@ -9486,16 +9482,16 @@
       <c r="AM90" s="13"/>
     </row>
     <row r="91" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A91" s="30" t="s">
+      <c r="A91" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B91" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="B91" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="C91" s="32">
+      <c r="C91" s="30">
         <v>8.5</v>
       </c>
-      <c r="D91" s="33">
+      <c r="D91" s="31">
         <v>606</v>
       </c>
       <c r="F91" s="13" t="str">
@@ -9633,373 +9629,373 @@
       <c r="AM91" s="13"/>
     </row>
     <row r="92" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A92" s="34" t="s">
+      <c r="A92" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B92" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="B92" s="35" t="s">
+      <c r="C92" s="34">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D92" s="35">
+        <v>1222</v>
+      </c>
+      <c r="F92" s="36"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="36"/>
+      <c r="I92" s="36"/>
+      <c r="J92" s="36"/>
+      <c r="K92" s="36"/>
+      <c r="L92" s="36"/>
+      <c r="M92" s="36"/>
+      <c r="N92" s="36"/>
+      <c r="O92" s="36"/>
+      <c r="P92" s="36"/>
+      <c r="Q92" s="36"/>
+      <c r="R92" s="36"/>
+      <c r="S92" s="36"/>
+      <c r="T92" s="36"/>
+      <c r="U92" s="36"/>
+      <c r="V92" s="36"/>
+      <c r="W92" s="36"/>
+      <c r="X92" s="36"/>
+      <c r="Y92" s="36"/>
+      <c r="Z92" s="36"/>
+      <c r="AA92" s="36"/>
+      <c r="AB92" s="36"/>
+      <c r="AC92" s="36"/>
+      <c r="AD92" s="36"/>
+      <c r="AE92" s="36"/>
+      <c r="AF92" s="36"/>
+      <c r="AG92" s="36"/>
+      <c r="AH92" s="36"/>
+      <c r="AI92" s="36"/>
+      <c r="AJ92" s="36"/>
+      <c r="AK92" s="36"/>
+      <c r="AL92" s="36"/>
+      <c r="AM92" s="36"/>
+    </row>
+    <row r="93" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A93" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="C92" s="36">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="D92" s="37">
-        <v>1222</v>
-      </c>
-      <c r="F92" s="38"/>
-      <c r="G92" s="38"/>
-      <c r="H92" s="38"/>
-      <c r="I92" s="38"/>
-      <c r="J92" s="38"/>
-      <c r="K92" s="38"/>
-      <c r="L92" s="38"/>
-      <c r="M92" s="38"/>
-      <c r="N92" s="38"/>
-      <c r="O92" s="38"/>
-      <c r="P92" s="38"/>
-      <c r="Q92" s="38"/>
-      <c r="R92" s="38"/>
-      <c r="S92" s="38"/>
-      <c r="T92" s="38"/>
-      <c r="U92" s="38"/>
-      <c r="V92" s="38"/>
-      <c r="W92" s="38"/>
-      <c r="X92" s="38"/>
-      <c r="Y92" s="38"/>
-      <c r="Z92" s="38"/>
-      <c r="AA92" s="38"/>
-      <c r="AB92" s="38"/>
-      <c r="AC92" s="38"/>
-      <c r="AD92" s="38"/>
-      <c r="AE92" s="38"/>
-      <c r="AF92" s="38"/>
-      <c r="AG92" s="38"/>
-      <c r="AH92" s="38"/>
-      <c r="AI92" s="38"/>
-      <c r="AJ92" s="38"/>
-      <c r="AK92" s="38"/>
-      <c r="AL92" s="38"/>
-      <c r="AM92" s="38"/>
-    </row>
-    <row r="93" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A93" s="30" t="s">
+      <c r="B93" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="B93" s="32" t="s">
+      <c r="C93" s="30">
+        <v>7.8</v>
+      </c>
+      <c r="D93" s="31">
+        <v>2404</v>
+      </c>
+      <c r="F93" s="36"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="36"/>
+      <c r="I93" s="36"/>
+      <c r="J93" s="36"/>
+      <c r="K93" s="36"/>
+      <c r="L93" s="36"/>
+      <c r="M93" s="36"/>
+      <c r="N93" s="36"/>
+      <c r="O93" s="36"/>
+      <c r="P93" s="36"/>
+      <c r="Q93" s="36"/>
+      <c r="R93" s="36"/>
+      <c r="S93" s="36"/>
+      <c r="T93" s="36"/>
+      <c r="U93" s="36"/>
+      <c r="V93" s="36"/>
+      <c r="W93" s="36"/>
+      <c r="X93" s="36"/>
+      <c r="Y93" s="36"/>
+      <c r="Z93" s="36"/>
+      <c r="AA93" s="36"/>
+      <c r="AB93" s="36"/>
+      <c r="AC93" s="36"/>
+      <c r="AD93" s="36"/>
+      <c r="AE93" s="36"/>
+      <c r="AF93" s="36"/>
+      <c r="AG93" s="36"/>
+      <c r="AH93" s="36"/>
+      <c r="AI93" s="36"/>
+      <c r="AJ93" s="36"/>
+      <c r="AK93" s="36"/>
+      <c r="AL93" s="36"/>
+      <c r="AM93" s="36"/>
+    </row>
+    <row r="94" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A94" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="C93" s="32">
-        <v>7.8</v>
-      </c>
-      <c r="D93" s="33">
-        <v>2404</v>
-      </c>
-      <c r="F93" s="38"/>
-      <c r="G93" s="38"/>
-      <c r="H93" s="38"/>
-      <c r="I93" s="38"/>
-      <c r="J93" s="38"/>
-      <c r="K93" s="38"/>
-      <c r="L93" s="38"/>
-      <c r="M93" s="38"/>
-      <c r="N93" s="38"/>
-      <c r="O93" s="38"/>
-      <c r="P93" s="38"/>
-      <c r="Q93" s="38"/>
-      <c r="R93" s="38"/>
-      <c r="S93" s="38"/>
-      <c r="T93" s="38"/>
-      <c r="U93" s="38"/>
-      <c r="V93" s="38"/>
-      <c r="W93" s="38"/>
-      <c r="X93" s="38"/>
-      <c r="Y93" s="38"/>
-      <c r="Z93" s="38"/>
-      <c r="AA93" s="38"/>
-      <c r="AB93" s="38"/>
-      <c r="AC93" s="38"/>
-      <c r="AD93" s="38"/>
-      <c r="AE93" s="38"/>
-      <c r="AF93" s="38"/>
-      <c r="AG93" s="38"/>
-      <c r="AH93" s="38"/>
-      <c r="AI93" s="38"/>
-      <c r="AJ93" s="38"/>
-      <c r="AK93" s="38"/>
-      <c r="AL93" s="38"/>
-      <c r="AM93" s="38"/>
-    </row>
-    <row r="94" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A94" s="34" t="s">
+      <c r="B94" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="B94" s="35" t="s">
+      <c r="C94" s="34">
+        <v>7.4</v>
+      </c>
+      <c r="D94" s="35">
+        <v>2444</v>
+      </c>
+      <c r="F94" s="36"/>
+      <c r="G94" s="36"/>
+      <c r="H94" s="36"/>
+      <c r="I94" s="36"/>
+      <c r="J94" s="36"/>
+      <c r="K94" s="36"/>
+      <c r="L94" s="36"/>
+      <c r="M94" s="36"/>
+      <c r="N94" s="36"/>
+      <c r="O94" s="36"/>
+      <c r="P94" s="36"/>
+      <c r="Q94" s="36"/>
+      <c r="R94" s="36"/>
+      <c r="S94" s="36"/>
+      <c r="T94" s="36"/>
+      <c r="U94" s="36"/>
+      <c r="V94" s="36"/>
+      <c r="W94" s="36"/>
+      <c r="X94" s="36"/>
+      <c r="Y94" s="36"/>
+      <c r="Z94" s="36"/>
+      <c r="AA94" s="36"/>
+      <c r="AB94" s="36"/>
+      <c r="AC94" s="36"/>
+      <c r="AD94" s="36"/>
+      <c r="AE94" s="36"/>
+      <c r="AF94" s="36"/>
+      <c r="AG94" s="36"/>
+      <c r="AH94" s="36"/>
+      <c r="AI94" s="36"/>
+      <c r="AJ94" s="36"/>
+      <c r="AK94" s="36"/>
+      <c r="AL94" s="36"/>
+      <c r="AM94" s="36"/>
+    </row>
+    <row r="95" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A95" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="C94" s="36">
-        <v>7.4</v>
-      </c>
-      <c r="D94" s="37">
-        <v>2444</v>
-      </c>
-      <c r="F94" s="38"/>
-      <c r="G94" s="38"/>
-      <c r="H94" s="38"/>
-      <c r="I94" s="38"/>
-      <c r="J94" s="38"/>
-      <c r="K94" s="38"/>
-      <c r="L94" s="38"/>
-      <c r="M94" s="38"/>
-      <c r="N94" s="38"/>
-      <c r="O94" s="38"/>
-      <c r="P94" s="38"/>
-      <c r="Q94" s="38"/>
-      <c r="R94" s="38"/>
-      <c r="S94" s="38"/>
-      <c r="T94" s="38"/>
-      <c r="U94" s="38"/>
-      <c r="V94" s="38"/>
-      <c r="W94" s="38"/>
-      <c r="X94" s="38"/>
-      <c r="Y94" s="38"/>
-      <c r="Z94" s="38"/>
-      <c r="AA94" s="38"/>
-      <c r="AB94" s="38"/>
-      <c r="AC94" s="38"/>
-      <c r="AD94" s="38"/>
-      <c r="AE94" s="38"/>
-      <c r="AF94" s="38"/>
-      <c r="AG94" s="38"/>
-      <c r="AH94" s="38"/>
-      <c r="AI94" s="38"/>
-      <c r="AJ94" s="38"/>
-      <c r="AK94" s="38"/>
-      <c r="AL94" s="38"/>
-      <c r="AM94" s="38"/>
-    </row>
-    <row r="95" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A95" s="30" t="s">
+      <c r="B95" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="B95" s="31" t="s">
+      <c r="C95" s="30">
+        <v>6.8</v>
+      </c>
+      <c r="D95" s="31">
+        <v>2441</v>
+      </c>
+      <c r="F95" s="36"/>
+      <c r="G95" s="36"/>
+      <c r="H95" s="36"/>
+      <c r="I95" s="36"/>
+      <c r="J95" s="36"/>
+      <c r="K95" s="36"/>
+      <c r="L95" s="36"/>
+      <c r="M95" s="36"/>
+      <c r="N95" s="36"/>
+      <c r="O95" s="36"/>
+      <c r="P95" s="36"/>
+      <c r="Q95" s="36"/>
+      <c r="R95" s="36"/>
+      <c r="S95" s="36"/>
+      <c r="T95" s="36"/>
+      <c r="U95" s="36"/>
+      <c r="V95" s="36"/>
+      <c r="W95" s="36"/>
+      <c r="X95" s="36"/>
+      <c r="Y95" s="36"/>
+      <c r="Z95" s="36"/>
+      <c r="AA95" s="36"/>
+      <c r="AB95" s="36"/>
+      <c r="AC95" s="36"/>
+      <c r="AD95" s="36"/>
+      <c r="AE95" s="36"/>
+      <c r="AF95" s="36"/>
+      <c r="AG95" s="36"/>
+      <c r="AH95" s="36"/>
+      <c r="AI95" s="36"/>
+      <c r="AJ95" s="36"/>
+      <c r="AK95" s="36"/>
+      <c r="AL95" s="36"/>
+      <c r="AM95" s="36"/>
+    </row>
+    <row r="96" spans="1:39" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="C95" s="32">
-        <v>6.8</v>
-      </c>
-      <c r="D95" s="33">
-        <v>2441</v>
-      </c>
-      <c r="F95" s="38"/>
-      <c r="G95" s="38"/>
-      <c r="H95" s="38"/>
-      <c r="I95" s="38"/>
-      <c r="J95" s="38"/>
-      <c r="K95" s="38"/>
-      <c r="L95" s="38"/>
-      <c r="M95" s="38"/>
-      <c r="N95" s="38"/>
-      <c r="O95" s="38"/>
-      <c r="P95" s="38"/>
-      <c r="Q95" s="38"/>
-      <c r="R95" s="38"/>
-      <c r="S95" s="38"/>
-      <c r="T95" s="38"/>
-      <c r="U95" s="38"/>
-      <c r="V95" s="38"/>
-      <c r="W95" s="38"/>
-      <c r="X95" s="38"/>
-      <c r="Y95" s="38"/>
-      <c r="Z95" s="38"/>
-      <c r="AA95" s="38"/>
-      <c r="AB95" s="38"/>
-      <c r="AC95" s="38"/>
-      <c r="AD95" s="38"/>
-      <c r="AE95" s="38"/>
-      <c r="AF95" s="38"/>
-      <c r="AG95" s="38"/>
-      <c r="AH95" s="38"/>
-      <c r="AI95" s="38"/>
-      <c r="AJ95" s="38"/>
-      <c r="AK95" s="38"/>
-      <c r="AL95" s="38"/>
-      <c r="AM95" s="38"/>
-    </row>
-    <row r="96" spans="1:39" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="34" t="s">
+      <c r="B96" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B96" s="35" t="s">
+      <c r="C96" s="34">
+        <v>6.2</v>
+      </c>
+      <c r="D96" s="35">
+        <v>2406</v>
+      </c>
+      <c r="F96" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="C96" s="36">
-        <v>6.2</v>
-      </c>
-      <c r="D96" s="37">
-        <v>2406</v>
-      </c>
-      <c r="F96" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="G96" s="38">
+      <c r="G96" s="36">
         <f>SUMPRODUCT(G88:G91,$D$88:$D$91)/SUM($D$88:$D$91)</f>
         <v>0</v>
       </c>
-      <c r="H96" s="38">
+      <c r="H96" s="36">
         <f t="shared" ref="H96:AM96" si="7">SUMPRODUCT(H88:H91,$D$88:$D$91)/SUM($D$88:$D$91)</f>
         <v>0.44754485596707821</v>
       </c>
-      <c r="I96" s="38">
+      <c r="I96" s="36">
         <f t="shared" si="7"/>
         <v>0.45145469983539099</v>
       </c>
-      <c r="J96" s="38">
+      <c r="J96" s="36">
         <f t="shared" si="7"/>
         <v>0.45536454370370372</v>
       </c>
-      <c r="K96" s="38">
+      <c r="K96" s="36">
         <f t="shared" si="7"/>
         <v>0.4592743875720165</v>
       </c>
-      <c r="L96" s="38">
+      <c r="L96" s="36">
         <f t="shared" si="7"/>
         <v>0.46318423144032922</v>
       </c>
-      <c r="M96" s="38">
+      <c r="M96" s="36">
         <f t="shared" si="7"/>
         <v>0.46709407530864194</v>
       </c>
-      <c r="N96" s="38">
+      <c r="N96" s="36">
         <f t="shared" si="7"/>
         <v>0.47100391917695472</v>
       </c>
-      <c r="O96" s="38">
+      <c r="O96" s="36">
         <f t="shared" si="7"/>
         <v>0.47491376304526756</v>
       </c>
-      <c r="P96" s="38">
+      <c r="P96" s="36">
         <f t="shared" si="7"/>
         <v>0.47882360691358022</v>
       </c>
-      <c r="Q96" s="38">
+      <c r="Q96" s="36">
         <f t="shared" si="7"/>
         <v>0.48273345078189311</v>
       </c>
-      <c r="R96" s="38">
+      <c r="R96" s="36">
         <f t="shared" si="7"/>
         <v>0.48664329465020567</v>
       </c>
-      <c r="S96" s="38">
+      <c r="S96" s="36">
         <f t="shared" si="7"/>
         <v>0.48713888179547321</v>
       </c>
-      <c r="T96" s="38">
+      <c r="T96" s="36">
         <f t="shared" si="7"/>
         <v>0.4876344689407407</v>
       </c>
-      <c r="U96" s="38">
+      <c r="U96" s="36">
         <f t="shared" si="7"/>
         <v>0.48813005608600823</v>
       </c>
-      <c r="V96" s="38">
+      <c r="V96" s="36">
         <f t="shared" si="7"/>
         <v>0.48862564323127572</v>
       </c>
-      <c r="W96" s="38">
+      <c r="W96" s="36">
         <f t="shared" si="7"/>
         <v>0.48912123037654326</v>
       </c>
-      <c r="X96" s="38">
+      <c r="X96" s="36">
         <f t="shared" si="7"/>
         <v>0.48961681752181074</v>
       </c>
-      <c r="Y96" s="38">
+      <c r="Y96" s="36">
         <f t="shared" si="7"/>
         <v>0.49011240466707828</v>
       </c>
-      <c r="Z96" s="38">
+      <c r="Z96" s="36">
         <f t="shared" si="7"/>
         <v>0.49060799181234577</v>
       </c>
-      <c r="AA96" s="38">
+      <c r="AA96" s="36">
         <f t="shared" si="7"/>
         <v>0.49110357895761308</v>
       </c>
-      <c r="AB96" s="38">
+      <c r="AB96" s="36">
         <f t="shared" si="7"/>
         <v>0.49159916610288062</v>
       </c>
-      <c r="AC96" s="38">
+      <c r="AC96" s="36">
         <f t="shared" si="7"/>
         <v>0.49209475324814811</v>
       </c>
-      <c r="AD96" s="38">
+      <c r="AD96" s="36">
         <f t="shared" si="7"/>
         <v>0.49259034039341565</v>
       </c>
-      <c r="AE96" s="38">
+      <c r="AE96" s="36">
         <f t="shared" si="7"/>
         <v>0.49308592753868313</v>
       </c>
-      <c r="AF96" s="38">
+      <c r="AF96" s="36">
         <f t="shared" si="7"/>
         <v>0.49358151468395067</v>
       </c>
-      <c r="AG96" s="38">
+      <c r="AG96" s="36">
         <f t="shared" si="7"/>
         <v>0.4940771018292181</v>
       </c>
-      <c r="AH96" s="38">
+      <c r="AH96" s="36">
         <f t="shared" si="7"/>
         <v>0.4945726889744857</v>
       </c>
-      <c r="AI96" s="38">
+      <c r="AI96" s="36">
         <f t="shared" si="7"/>
         <v>0.49506827611975313</v>
       </c>
-      <c r="AJ96" s="38">
+      <c r="AJ96" s="36">
         <f t="shared" si="7"/>
         <v>0.4955638632650205</v>
       </c>
-      <c r="AK96" s="38">
+      <c r="AK96" s="36">
         <f t="shared" si="7"/>
         <v>0.49605945041028804</v>
       </c>
-      <c r="AL96" s="38">
+      <c r="AL96" s="36">
         <f t="shared" si="7"/>
         <v>0.49655503755555552</v>
       </c>
-      <c r="AM96" s="38">
+      <c r="AM96" s="36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="40" t="s">
+      <c r="A97" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B97" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="B97" s="41" t="s">
+      <c r="C97" s="40">
+        <v>5.2</v>
+      </c>
+      <c r="D97" s="41">
+        <v>3044</v>
+      </c>
+    </row>
+    <row r="98" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="C97" s="42">
-        <v>5.2</v>
-      </c>
-      <c r="D97" s="43">
-        <v>3044</v>
-      </c>
-    </row>
-    <row r="98" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="44" t="s">
-        <v>128</v>
-      </c>
-      <c r="B98" s="45"/>
-      <c r="C98" s="45"/>
-      <c r="D98" s="46">
+      <c r="B98" s="43"/>
+      <c r="C98" s="43"/>
+      <c r="D98" s="44">
         <v>15176</v>
       </c>
     </row>
     <row r="100" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -10134,7 +10130,7 @@
     </row>
     <row r="102" spans="1:34" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B102" s="15"/>
       <c r="C102" s="15">
@@ -10233,7 +10229,7 @@
     </row>
     <row r="103" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B103" s="16"/>
       <c r="C103" s="16">
@@ -10332,7 +10328,7 @@
     </row>
     <row r="104" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B104" s="18"/>
       <c r="C104" s="18">
@@ -10431,7 +10427,7 @@
     </row>
     <row r="105" spans="1:34" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B105" s="15"/>
       <c r="C105" s="15">
@@ -10530,7 +10526,7 @@
     </row>
     <row r="106" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B106" s="16"/>
       <c r="C106" s="16">
@@ -10629,7 +10625,7 @@
     </row>
     <row r="107" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B107" s="18"/>
       <c r="C107" s="18">
@@ -10728,7 +10724,7 @@
     </row>
     <row r="108" spans="1:34" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B108" s="15"/>
       <c r="C108" s="15">
@@ -10764,7 +10760,7 @@
       <c r="M108" s="15">
         <v>0.51842377106021331</v>
       </c>
-      <c r="N108" s="47">
+      <c r="N108" s="45">
         <v>0.5210607852037108</v>
       </c>
       <c r="O108" s="15">
@@ -10827,7 +10823,7 @@
     </row>
     <row r="109" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B109" s="16"/>
       <c r="C109" s="16">
@@ -10863,7 +10859,7 @@
       <c r="M109" s="16">
         <v>0.50020117891032945</v>
       </c>
-      <c r="N109" s="48">
+      <c r="N109" s="46">
         <v>0.50233715870636042</v>
       </c>
       <c r="O109" s="16">
@@ -10926,7 +10922,7 @@
     </row>
     <row r="110" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B110" s="18"/>
       <c r="C110" s="18">
@@ -10962,7 +10958,7 @@
       <c r="M110" s="18">
         <v>0.46017400743379333</v>
       </c>
-      <c r="N110" s="49">
+      <c r="N110" s="47">
         <v>0.46121780506774213</v>
       </c>
       <c r="O110" s="18">
@@ -11025,7 +11021,7 @@
     </row>
     <row r="111" spans="1:34" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B111" s="15"/>
       <c r="C111" s="15">
@@ -11124,7 +11120,7 @@
     </row>
     <row r="112" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B112" s="16"/>
       <c r="C112" s="16">
@@ -11223,7 +11219,7 @@
     </row>
     <row r="113" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B113" s="18"/>
       <c r="C113" s="18">
@@ -11322,7 +11318,7 @@
     </row>
     <row r="114" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B114" s="15"/>
       <c r="C114" s="15">
@@ -11421,7 +11417,7 @@
     </row>
     <row r="115" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B115" s="16"/>
       <c r="C115" s="16">
@@ -11520,7 +11516,7 @@
     </row>
     <row r="116" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B116" s="18"/>
       <c r="C116" s="18">
@@ -11619,7 +11615,7 @@
     </row>
     <row r="117" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B117" s="15"/>
       <c r="C117" s="15">
@@ -11718,7 +11714,7 @@
     </row>
     <row r="118" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B118" s="16"/>
       <c r="C118" s="16">
@@ -11817,7 +11813,7 @@
     </row>
     <row r="119" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B119" s="18"/>
       <c r="C119" s="18">
@@ -11916,7 +11912,7 @@
     </row>
     <row r="120" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B120" s="15"/>
       <c r="C120" s="15">
@@ -12015,7 +12011,7 @@
     </row>
     <row r="121" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B121" s="16"/>
       <c r="C121" s="16">
@@ -12114,7 +12110,7 @@
     </row>
     <row r="122" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B122" s="18"/>
       <c r="C122" s="18">
@@ -12213,7 +12209,7 @@
     </row>
     <row r="123" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B123" s="15"/>
       <c r="C123" s="15">
@@ -12312,7 +12308,7 @@
     </row>
     <row r="124" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B124" s="16"/>
       <c r="C124" s="16">
@@ -12411,7 +12407,7 @@
     </row>
     <row r="125" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B125" s="18"/>
       <c r="C125" s="18">
@@ -12510,7 +12506,7 @@
     </row>
     <row r="126" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B126" s="15"/>
       <c r="C126" s="15">
@@ -12609,7 +12605,7 @@
     </row>
     <row r="127" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B127" s="16"/>
       <c r="C127" s="16">
@@ -12708,7 +12704,7 @@
     </row>
     <row r="128" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B128" s="18"/>
       <c r="C128" s="18">
@@ -12807,7 +12803,7 @@
     </row>
     <row r="129" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B129" s="15"/>
       <c r="C129" s="15">
@@ -12906,7 +12902,7 @@
     </row>
     <row r="130" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B130" s="16"/>
       <c r="C130" s="16">
@@ -13005,7 +13001,7 @@
     </row>
     <row r="131" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B131" s="18"/>
       <c r="C131" s="18">
@@ -13104,7 +13100,7 @@
     </row>
     <row r="132" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B132" s="15"/>
       <c r="C132" s="15">
@@ -13203,7 +13199,7 @@
     </row>
     <row r="133" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133" s="16"/>
       <c r="C133" s="16">
@@ -13302,7 +13298,7 @@
     </row>
     <row r="134" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B134" s="18"/>
       <c r="C134" s="18">
@@ -13401,7 +13397,7 @@
     </row>
     <row r="135" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B135" s="15"/>
       <c r="C135" s="15">
@@ -13500,7 +13496,7 @@
     </row>
     <row r="136" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B136" s="16"/>
       <c r="C136" s="16">
@@ -13599,7 +13595,7 @@
     </row>
     <row r="137" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B137" s="18"/>
       <c r="C137" s="18">
@@ -13698,7 +13694,7 @@
     </row>
     <row r="138" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B138" s="15"/>
       <c r="C138" s="15">
@@ -13734,7 +13730,7 @@
       <c r="M138" s="15">
         <v>0.41904719232527327</v>
       </c>
-      <c r="N138" s="47">
+      <c r="N138" s="45">
         <v>0.42078032078848659</v>
       </c>
       <c r="O138" s="15">
@@ -13797,7 +13793,7 @@
     </row>
     <row r="139" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B139" s="16"/>
       <c r="C139" s="16">
@@ -13833,7 +13829,7 @@
       <c r="M139" s="16">
         <v>0.40622711298112724</v>
       </c>
-      <c r="N139" s="48">
+      <c r="N139" s="46">
         <v>0.40762672467107541</v>
       </c>
       <c r="O139" s="16">
@@ -13896,7 +13892,7 @@
     </row>
     <row r="140" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B140" s="18"/>
       <c r="C140" s="18">
@@ -13932,7 +13928,7 @@
       <c r="M140" s="18">
         <v>0.3792558660822587</v>
       </c>
-      <c r="N140" s="49">
+      <c r="N140" s="47">
         <v>0.37995196965318284</v>
       </c>
       <c r="O140" s="18">
@@ -13995,7 +13991,7 @@
     </row>
     <row r="141" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A141" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B141" s="15"/>
       <c r="C141" s="15">
@@ -14094,7 +14090,7 @@
     </row>
     <row r="142" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B142" s="16"/>
       <c r="C142" s="16">
@@ -14193,7 +14189,7 @@
     </row>
     <row r="143" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A143" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B143" s="18"/>
       <c r="C143" s="18">
@@ -14292,105 +14288,105 @@
     </row>
     <row r="148" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>142</v>
-      </c>
-      <c r="F148" s="50">
+        <v>141</v>
+      </c>
+      <c r="F148" s="48">
         <v>2020</v>
       </c>
-      <c r="G148" s="50">
+      <c r="G148" s="48">
         <v>2021</v>
       </c>
-      <c r="H148" s="50">
+      <c r="H148" s="48">
         <v>2022</v>
       </c>
-      <c r="I148" s="50">
+      <c r="I148" s="48">
         <v>2023</v>
       </c>
-      <c r="J148" s="50">
+      <c r="J148" s="48">
         <v>2024</v>
       </c>
-      <c r="K148" s="50">
+      <c r="K148" s="48">
         <v>2025</v>
       </c>
-      <c r="L148" s="50">
+      <c r="L148" s="48">
         <v>2026</v>
       </c>
-      <c r="M148" s="50">
+      <c r="M148" s="48">
         <v>2027</v>
       </c>
-      <c r="N148" s="50">
+      <c r="N148" s="48">
         <v>2028</v>
       </c>
-      <c r="O148" s="50">
+      <c r="O148" s="48">
         <v>2029</v>
       </c>
-      <c r="P148" s="50">
+      <c r="P148" s="48">
         <v>2030</v>
       </c>
-      <c r="Q148" s="50">
+      <c r="Q148" s="48">
         <v>2031</v>
       </c>
-      <c r="R148" s="50">
+      <c r="R148" s="48">
         <v>2032</v>
       </c>
-      <c r="S148" s="50">
+      <c r="S148" s="48">
         <v>2033</v>
       </c>
-      <c r="T148" s="50">
+      <c r="T148" s="48">
         <v>2034</v>
       </c>
-      <c r="U148" s="50">
+      <c r="U148" s="48">
         <v>2035</v>
       </c>
-      <c r="V148" s="50">
+      <c r="V148" s="48">
         <v>2036</v>
       </c>
-      <c r="W148" s="50">
+      <c r="W148" s="48">
         <v>2037</v>
       </c>
-      <c r="X148" s="50">
+      <c r="X148" s="48">
         <v>2038</v>
       </c>
-      <c r="Y148" s="50">
+      <c r="Y148" s="48">
         <v>2039</v>
       </c>
-      <c r="Z148" s="50">
+      <c r="Z148" s="48">
         <v>2040</v>
       </c>
-      <c r="AA148" s="50">
+      <c r="AA148" s="48">
         <v>2041</v>
       </c>
-      <c r="AB148" s="50">
+      <c r="AB148" s="48">
         <v>2042</v>
       </c>
-      <c r="AC148" s="50">
+      <c r="AC148" s="48">
         <v>2043</v>
       </c>
-      <c r="AD148" s="50">
+      <c r="AD148" s="48">
         <v>2044</v>
       </c>
-      <c r="AE148" s="50">
+      <c r="AE148" s="48">
         <v>2045</v>
       </c>
-      <c r="AF148" s="50">
+      <c r="AF148" s="48">
         <v>2046</v>
       </c>
-      <c r="AG148" s="50">
+      <c r="AG148" s="48">
         <v>2047</v>
       </c>
-      <c r="AH148" s="50">
+      <c r="AH148" s="48">
         <v>2048</v>
       </c>
-      <c r="AI148" s="50">
+      <c r="AI148" s="48">
         <v>2049</v>
       </c>
-      <c r="AJ148" s="50">
+      <c r="AJ148" s="48">
         <v>2050</v>
       </c>
     </row>
     <row r="149" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B149">
         <v>13.57</v>
@@ -14530,7 +14526,7 @@
     </row>
     <row r="150" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B150">
         <v>13.57</v>
@@ -14670,7 +14666,7 @@
     </row>
     <row r="151" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B151">
         <v>27.6</v>
@@ -14810,7 +14806,7 @@
     </row>
     <row r="152" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B152">
         <v>27.6</v>
@@ -14949,8 +14945,8 @@
       </c>
     </row>
     <row r="154" spans="1:38" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="D154" s="51" t="s">
-        <v>147</v>
+      <c r="D154" s="49" t="s">
+        <v>146</v>
       </c>
       <c r="E154" s="13">
         <f>SUMPRODUCT(E149:E152,$B$149:$B$152)/SUM($B$149:$B$152)</f>
@@ -15102,14 +15098,12 @@
   </sheetPr>
   <dimension ref="A1:AF18"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:AF11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -15209,7 +15203,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -15307,7 +15301,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -15405,7 +15399,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -15503,7 +15497,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -15601,7 +15595,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -15699,263 +15693,263 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7" s="52">
-        <f>'NREL ATB 2022'!I96/'NREL ATB 2022'!H96-1</f>
+      <c r="C7" s="55">
+        <f>'NREL ATB 2022'!I96/'NREL ATB 2022'!$H96-1</f>
         <v>8.7362055806992078E-3</v>
       </c>
-      <c r="D7" s="52">
-        <f>'NREL ATB 2022'!J96/'NREL ATB 2022'!I96-1</f>
-        <v>8.6605452767205549E-3</v>
-      </c>
-      <c r="E7" s="52">
-        <f>'NREL ATB 2022'!K96/'NREL ATB 2022'!J96-1</f>
-        <v>8.5861842393615273E-3</v>
-      </c>
-      <c r="F7" s="52">
-        <f>'NREL ATB 2022'!L96/'NREL ATB 2022'!K96-1</f>
-        <v>8.5130892863030105E-3</v>
-      </c>
-      <c r="G7" s="52">
-        <f>'NREL ATB 2022'!M96/'NREL ATB 2022'!L96-1</f>
-        <v>8.4412283556254408E-3</v>
-      </c>
-      <c r="H7" s="52">
-        <f>'NREL ATB 2022'!N96/'NREL ATB 2022'!M96-1</f>
-        <v>8.3705704589149832E-3</v>
-      </c>
-      <c r="I7" s="52">
-        <f>'NREL ATB 2022'!O96/'NREL ATB 2022'!N96-1</f>
-        <v>8.3010856367076169E-3</v>
-      </c>
-      <c r="J7" s="52">
-        <f>'NREL ATB 2022'!P96/'NREL ATB 2022'!O96-1</f>
-        <v>8.2327449161332389E-3</v>
-      </c>
-      <c r="K7" s="52">
-        <f>'NREL ATB 2022'!Q96/'NREL ATB 2022'!P96-1</f>
-        <v>8.1655202706381047E-3</v>
-      </c>
-      <c r="L7" s="52">
-        <f>'NREL ATB 2022'!R96/'NREL ATB 2022'!Q96-1</f>
-        <v>8.0993845816561549E-3</v>
-      </c>
-      <c r="M7" s="52">
-        <f>'NREL ATB 2022'!S96/'NREL ATB 2022'!R96-1</f>
-        <v>1.0183786578705778E-3</v>
-      </c>
-      <c r="N7" s="52">
-        <f>'NREL ATB 2022'!T96/'NREL ATB 2022'!S96-1</f>
-        <v>1.0173426178605727E-3</v>
-      </c>
-      <c r="O7" s="52">
-        <f>'NREL ATB 2022'!U96/'NREL ATB 2022'!T96-1</f>
-        <v>1.0163086837238211E-3</v>
-      </c>
-      <c r="P7" s="52">
-        <f>'NREL ATB 2022'!V96/'NREL ATB 2022'!U96-1</f>
-        <v>1.0152768490456765E-3</v>
-      </c>
-      <c r="Q7" s="52">
-        <f>'NREL ATB 2022'!W96/'NREL ATB 2022'!V96-1</f>
-        <v>1.0142471074383597E-3</v>
-      </c>
-      <c r="R7" s="52">
-        <f>'NREL ATB 2022'!X96/'NREL ATB 2022'!W96-1</f>
-        <v>1.0132194525394045E-3</v>
-      </c>
-      <c r="S7" s="52">
-        <f>'NREL ATB 2022'!Y96/'NREL ATB 2022'!X96-1</f>
-        <v>1.0121938780125461E-3</v>
-      </c>
-      <c r="T7" s="52">
-        <f>'NREL ATB 2022'!Z96/'NREL ATB 2022'!Y96-1</f>
-        <v>1.0111703775466108E-3</v>
-      </c>
-      <c r="U7" s="52">
-        <f>'NREL ATB 2022'!AA96/'NREL ATB 2022'!Z96-1</f>
-        <v>1.0101489448564038E-3</v>
-      </c>
-      <c r="V7" s="52">
-        <f>'NREL ATB 2022'!AB96/'NREL ATB 2022'!AA96-1</f>
-        <v>1.0091295736827099E-3</v>
-      </c>
-      <c r="W7" s="52">
-        <f>'NREL ATB 2022'!AC96/'NREL ATB 2022'!AB96-1</f>
-        <v>1.0081122577896284E-3</v>
-      </c>
-      <c r="X7" s="52">
-        <f>'NREL ATB 2022'!AD96/'NREL ATB 2022'!AC96-1</f>
-        <v>1.007096990968348E-3</v>
-      </c>
-      <c r="Y7" s="52">
-        <f>'NREL ATB 2022'!AE96/'NREL ATB 2022'!AD96-1</f>
-        <v>1.0060837670338163E-3</v>
-      </c>
-      <c r="Z7" s="52">
-        <f>'NREL ATB 2022'!AF96/'NREL ATB 2022'!AE96-1</f>
-        <v>1.0050725798267379E-3</v>
-      </c>
-      <c r="AA7" s="52">
-        <f>'NREL ATB 2022'!AG96/'NREL ATB 2022'!AF96-1</f>
-        <v>1.0040634232113543E-3</v>
-      </c>
-      <c r="AB7" s="52">
-        <f>'NREL ATB 2022'!AH96/'NREL ATB 2022'!AG96-1</f>
-        <v>1.0030562910783303E-3</v>
-      </c>
-      <c r="AC7" s="52">
-        <f>'NREL ATB 2022'!AI96/'NREL ATB 2022'!AH96-1</f>
-        <v>1.002051177340757E-3</v>
-      </c>
-      <c r="AD7" s="52">
-        <f>'NREL ATB 2022'!AJ96/'NREL ATB 2022'!AI96-1</f>
-        <v>1.0010480759374829E-3</v>
-      </c>
-      <c r="AE7" s="52">
-        <f>'NREL ATB 2022'!AK96/'NREL ATB 2022'!AJ96-1</f>
-        <v>1.0000469808317813E-3</v>
-      </c>
-      <c r="AF7" s="52">
-        <f>'NREL ATB 2022'!AL96/'NREL ATB 2022'!AK96-1</f>
-        <v>9.9904788600957417E-4</v>
+      <c r="D7" s="55">
+        <f>'NREL ATB 2022'!J96/'NREL ATB 2022'!$H96-1</f>
+        <v>1.7472411161398194E-2</v>
+      </c>
+      <c r="E7" s="55">
+        <f>'NREL ATB 2022'!K96/'NREL ATB 2022'!$H96-1</f>
+        <v>2.6208616742097179E-2</v>
+      </c>
+      <c r="F7" s="55">
+        <f>'NREL ATB 2022'!L96/'NREL ATB 2022'!$H96-1</f>
+        <v>3.4944822322796387E-2</v>
+      </c>
+      <c r="G7" s="55">
+        <f>'NREL ATB 2022'!M96/'NREL ATB 2022'!$H96-1</f>
+        <v>4.3681027903495373E-2</v>
+      </c>
+      <c r="H7" s="55">
+        <f>'NREL ATB 2022'!N96/'NREL ATB 2022'!$H96-1</f>
+        <v>5.2417233484194359E-2</v>
+      </c>
+      <c r="I7" s="55">
+        <f>'NREL ATB 2022'!O96/'NREL ATB 2022'!$H96-1</f>
+        <v>6.1153439064893789E-2</v>
+      </c>
+      <c r="J7" s="55">
+        <f>'NREL ATB 2022'!P96/'NREL ATB 2022'!$H96-1</f>
+        <v>6.9889644645592552E-2</v>
+      </c>
+      <c r="K7" s="55">
+        <f>'NREL ATB 2022'!Q96/'NREL ATB 2022'!$H96-1</f>
+        <v>7.8625850226291982E-2</v>
+      </c>
+      <c r="L7" s="55">
+        <f>'NREL ATB 2022'!R96/'NREL ATB 2022'!$H96-1</f>
+        <v>8.7362055806990524E-2</v>
+      </c>
+      <c r="M7" s="55">
+        <f>'NREL ATB 2022'!S96/'NREL ATB 2022'!$H96-1</f>
+        <v>8.8469402118002582E-2</v>
+      </c>
+      <c r="N7" s="55">
+        <f>'NREL ATB 2022'!T96/'NREL ATB 2022'!$H96-1</f>
+        <v>8.9576748429014419E-2</v>
+      </c>
+      <c r="O7" s="55">
+        <f>'NREL ATB 2022'!U96/'NREL ATB 2022'!$H96-1</f>
+        <v>9.0684094740026477E-2</v>
+      </c>
+      <c r="P7" s="55">
+        <f>'NREL ATB 2022'!V96/'NREL ATB 2022'!$H96-1</f>
+        <v>9.1791441051038314E-2</v>
+      </c>
+      <c r="Q7" s="55">
+        <f>'NREL ATB 2022'!W96/'NREL ATB 2022'!$H96-1</f>
+        <v>9.2898787362050372E-2</v>
+      </c>
+      <c r="R7" s="55">
+        <f>'NREL ATB 2022'!X96/'NREL ATB 2022'!$H96-1</f>
+        <v>9.4006133673062209E-2</v>
+      </c>
+      <c r="S7" s="55">
+        <f>'NREL ATB 2022'!Y96/'NREL ATB 2022'!$H96-1</f>
+        <v>9.5113479984074267E-2</v>
+      </c>
+      <c r="T7" s="55">
+        <f>'NREL ATB 2022'!Z96/'NREL ATB 2022'!$H96-1</f>
+        <v>9.6220826295086104E-2</v>
+      </c>
+      <c r="U7" s="55">
+        <f>'NREL ATB 2022'!AA96/'NREL ATB 2022'!$H96-1</f>
+        <v>9.7328172606097496E-2</v>
+      </c>
+      <c r="V7" s="55">
+        <f>'NREL ATB 2022'!AB96/'NREL ATB 2022'!$H96-1</f>
+        <v>9.8435518917109555E-2</v>
+      </c>
+      <c r="W7" s="55">
+        <f>'NREL ATB 2022'!AC96/'NREL ATB 2022'!$H96-1</f>
+        <v>9.9542865228121391E-2</v>
+      </c>
+      <c r="X7" s="55">
+        <f>'NREL ATB 2022'!AD96/'NREL ATB 2022'!$H96-1</f>
+        <v>0.10065021153913345</v>
+      </c>
+      <c r="Y7" s="55">
+        <f>'NREL ATB 2022'!AE96/'NREL ATB 2022'!$H96-1</f>
+        <v>0.10175755785014529</v>
+      </c>
+      <c r="Z7" s="55">
+        <f>'NREL ATB 2022'!AF96/'NREL ATB 2022'!$H96-1</f>
+        <v>0.10286490416115734</v>
+      </c>
+      <c r="AA7" s="55">
+        <f>'NREL ATB 2022'!AG96/'NREL ATB 2022'!$H96-1</f>
+        <v>0.10397225047216918</v>
+      </c>
+      <c r="AB7" s="55">
+        <f>'NREL ATB 2022'!AH96/'NREL ATB 2022'!$H96-1</f>
+        <v>0.10507959678318124</v>
+      </c>
+      <c r="AC7" s="55">
+        <f>'NREL ATB 2022'!AI96/'NREL ATB 2022'!$H96-1</f>
+        <v>0.10618694309419285</v>
+      </c>
+      <c r="AD7" s="55">
+        <f>'NREL ATB 2022'!AJ96/'NREL ATB 2022'!$H96-1</f>
+        <v>0.10729428940520447</v>
+      </c>
+      <c r="AE7" s="55">
+        <f>'NREL ATB 2022'!AK96/'NREL ATB 2022'!$H96-1</f>
+        <v>0.10840163571621653</v>
+      </c>
+      <c r="AF7" s="55">
+        <f>'NREL ATB 2022'!AL96/'NREL ATB 2022'!$H96-1</f>
+        <v>0.10950898202722836</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <f>'NREL ATB 2022'!D36/'NREL ATB 2022'!C36-1</f>
+        <f>'NREL ATB 2022'!D36/'NREL ATB 2022'!$C36-1</f>
         <v>9.5591208928909044E-3</v>
       </c>
       <c r="D8">
-        <f>'NREL ATB 2022'!E36/'NREL ATB 2022'!D36-1</f>
-        <v>9.4686093117919423E-3</v>
+        <f>'NREL ATB 2022'!E36/'NREL ATB 2022'!$C36-1</f>
+        <v>1.9118241785781809E-2</v>
       </c>
       <c r="E8">
-        <f>'NREL ATB 2022'!F36/'NREL ATB 2022'!E36-1</f>
-        <v>9.3797956909698055E-3</v>
+        <f>'NREL ATB 2022'!F36/'NREL ATB 2022'!$C36-1</f>
+        <v>2.8677362678672713E-2</v>
       </c>
       <c r="F8">
-        <f>'NREL ATB 2022'!G36/'NREL ATB 2022'!F36-1</f>
-        <v>9.2926326948608029E-3</v>
+        <f>'NREL ATB 2022'!G36/'NREL ATB 2022'!$C36-1</f>
+        <v>3.823648357156384E-2</v>
       </c>
       <c r="G8">
-        <f>'NREL ATB 2022'!H36/'NREL ATB 2022'!G36-1</f>
-        <v>9.2070747311892021E-3</v>
+        <f>'NREL ATB 2022'!H36/'NREL ATB 2022'!$C36-1</f>
+        <v>4.77956044644543E-2</v>
       </c>
       <c r="H8">
-        <f>'NREL ATB 2022'!I36/'NREL ATB 2022'!H36-1</f>
-        <v>9.1230778714492811E-3</v>
+        <f>'NREL ATB 2022'!I36/'NREL ATB 2022'!$C36-1</f>
+        <v>5.735472535734587E-2</v>
       </c>
       <c r="I8">
-        <f>'NREL ATB 2022'!J36/'NREL ATB 2022'!I36-1</f>
-        <v>9.0405997756903833E-3</v>
+        <f>'NREL ATB 2022'!J36/'NREL ATB 2022'!$C36-1</f>
+        <v>6.6913846250236553E-2</v>
       </c>
       <c r="J8">
-        <f>'NREL ATB 2022'!K36/'NREL ATB 2022'!J36-1</f>
-        <v>8.9595996213633899E-3</v>
+        <f>'NREL ATB 2022'!K36/'NREL ATB 2022'!$C36-1</f>
+        <v>7.6472967143127679E-2</v>
       </c>
       <c r="K8">
-        <f>'NREL ATB 2022'!L36/'NREL ATB 2022'!K36-1</f>
-        <v>8.88003803593862E-3</v>
+        <f>'NREL ATB 2022'!L36/'NREL ATB 2022'!$C36-1</f>
+        <v>8.6032088036018362E-2</v>
       </c>
       <c r="L8">
-        <f>'NREL ATB 2022'!M36/'NREL ATB 2022'!L36-1</f>
-        <v>8.8018770330973162E-3</v>
+        <f>'NREL ATB 2022'!M36/'NREL ATB 2022'!$C36-1</f>
+        <v>9.5591208928909488E-2</v>
       </c>
       <c r="M8">
-        <f>'NREL ATB 2022'!N36/'NREL ATB 2022'!M36-1</f>
-        <v>3.7959803427889405E-3</v>
+        <f>'NREL ATB 2022'!N36/'NREL ATB 2022'!$C36-1</f>
+        <v>9.975005162173578E-2</v>
       </c>
       <c r="N8">
-        <f>'NREL ATB 2022'!O36/'NREL ATB 2022'!N36-1</f>
-        <v>3.7816253672313671E-3</v>
+        <f>'NREL ATB 2022'!O36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.10390889431456252</v>
       </c>
       <c r="O8">
-        <f>'NREL ATB 2022'!P36/'NREL ATB 2022'!O36-1</f>
-        <v>3.767378552927525E-3</v>
+        <f>'NREL ATB 2022'!P36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.10806773700738925</v>
       </c>
       <c r="P8">
-        <f>'NREL ATB 2022'!Q36/'NREL ATB 2022'!P36-1</f>
-        <v>3.7532386820124941E-3</v>
+        <f>'NREL ATB 2022'!Q36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.11222657970021532</v>
       </c>
       <c r="Q8">
-        <f>'NREL ATB 2022'!R36/'NREL ATB 2022'!Q36-1</f>
-        <v>3.7392045548376718E-3</v>
+        <f>'NREL ATB 2022'!R36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.11638542239304206</v>
       </c>
       <c r="R8">
-        <f>'NREL ATB 2022'!S36/'NREL ATB 2022'!R36-1</f>
-        <v>3.7252749896286019E-3</v>
+        <f>'NREL ATB 2022'!S36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.1205442650858688</v>
       </c>
       <c r="S8">
-        <f>'NREL ATB 2022'!T36/'NREL ATB 2022'!S36-1</f>
-        <v>3.711448822155905E-3</v>
+        <f>'NREL ATB 2022'!T36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.12470310777869509</v>
       </c>
       <c r="T8">
-        <f>'NREL ATB 2022'!U36/'NREL ATB 2022'!T36-1</f>
-        <v>3.6977249054113148E-3</v>
+        <f>'NREL ATB 2022'!U36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.12886195047152182</v>
       </c>
       <c r="U8">
-        <f>'NREL ATB 2022'!V36/'NREL ATB 2022'!U36-1</f>
-        <v>3.6841021092877124E-3</v>
+        <f>'NREL ATB 2022'!V36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.13302079316434856</v>
       </c>
       <c r="V8">
-        <f>'NREL ATB 2022'!W36/'NREL ATB 2022'!V36-1</f>
-        <v>3.6705793202711501E-3</v>
+        <f>'NREL ATB 2022'!W36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.13717963585717463</v>
       </c>
       <c r="W8">
-        <f>'NREL ATB 2022'!X36/'NREL ATB 2022'!W36-1</f>
-        <v>3.6571554411382046E-3</v>
+        <f>'NREL ATB 2022'!X36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.14133847855000137</v>
       </c>
       <c r="X8">
-        <f>'NREL ATB 2022'!Y36/'NREL ATB 2022'!X36-1</f>
-        <v>3.6438293906557728E-3</v>
+        <f>'NREL ATB 2022'!Y36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.14549732124282833</v>
       </c>
       <c r="Y8">
-        <f>'NREL ATB 2022'!Z36/'NREL ATB 2022'!Y36-1</f>
-        <v>3.6306001032930801E-3</v>
+        <f>'NREL ATB 2022'!Z36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.1496561639356544</v>
       </c>
       <c r="Z8">
-        <f>'NREL ATB 2022'!AA36/'NREL ATB 2022'!Z36-1</f>
-        <v>3.6174665289399055E-3</v>
+        <f>'NREL ATB 2022'!AA36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.15381500662848113</v>
       </c>
       <c r="AA8">
-        <f>'NREL ATB 2022'!AB36/'NREL ATB 2022'!AA36-1</f>
-        <v>3.6044276326225866E-3</v>
+        <f>'NREL ATB 2022'!AB36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.15797384932130765</v>
       </c>
       <c r="AB8">
-        <f>'NREL ATB 2022'!AC36/'NREL ATB 2022'!AB36-1</f>
-        <v>3.5914823942391205E-3</v>
+        <f>'NREL ATB 2022'!AC36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.16213269201413438</v>
       </c>
       <c r="AC8">
-        <f>'NREL ATB 2022'!AD36/'NREL ATB 2022'!AC36-1</f>
-        <v>3.5786298082871593E-3</v>
+        <f>'NREL ATB 2022'!AD36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.16629153470696112</v>
       </c>
       <c r="AD8">
-        <f>'NREL ATB 2022'!AE36/'NREL ATB 2022'!AD36-1</f>
-        <v>3.5658688836077701E-3</v>
+        <f>'NREL ATB 2022'!AE36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.17045037739978786</v>
       </c>
       <c r="AE8">
-        <f>'NREL ATB 2022'!AF36/'NREL ATB 2022'!AE36-1</f>
-        <v>3.5531986431285301E-3</v>
+        <f>'NREL ATB 2022'!AF36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.17460922009261393</v>
       </c>
       <c r="AF8">
-        <f>'NREL ATB 2022'!AG36/'NREL ATB 2022'!AF36-1</f>
-        <v>3.5406181236163903E-3</v>
+        <f>'NREL ATB 2022'!AG36/'NREL ATB 2022'!$C36-1</f>
+        <v>0.17876806278544088</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -16053,7 +16047,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -16151,7 +16145,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -16249,7 +16243,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -16347,7 +16341,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -16445,7 +16439,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -16543,135 +16537,135 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
-      <c r="C15" s="52">
-        <f>'NREL ATB 2022'!G154/'NREL ATB 2022'!F154-1</f>
+      <c r="C15" s="55">
+        <f>'NREL ATB 2022'!G154/'NREL ATB 2022'!$F154-1</f>
         <v>1.2012960298790842E-2</v>
       </c>
-      <c r="D15" s="52">
-        <f>'NREL ATB 2022'!H154/'NREL ATB 2022'!G154-1</f>
-        <v>1.0559622683238956E-2</v>
-      </c>
-      <c r="E15" s="52">
-        <f>'NREL ATB 2022'!I154/'NREL ATB 2022'!H154-1</f>
-        <v>9.6288746872572606E-3</v>
-      </c>
-      <c r="F15" s="52">
-        <f>'NREL ATB 2022'!J154/'NREL ATB 2022'!I154-1</f>
-        <v>8.9762875765646566E-3</v>
-      </c>
-      <c r="G15" s="52">
-        <f>'NREL ATB 2022'!K154/'NREL ATB 2022'!J154-1</f>
-        <v>8.4896443386619502E-3</v>
-      </c>
-      <c r="H15" s="52">
-        <f>'NREL ATB 2022'!L154/'NREL ATB 2022'!K154-1</f>
-        <v>8.1101019818372588E-3</v>
-      </c>
-      <c r="I15" s="52">
-        <f>'NREL ATB 2022'!M154/'NREL ATB 2022'!L154-1</f>
-        <v>7.8037985715639913E-3</v>
-      </c>
-      <c r="J15" s="52">
-        <f>'NREL ATB 2022'!N154/'NREL ATB 2022'!M154-1</f>
-        <v>7.5498544261711764E-3</v>
-      </c>
-      <c r="K15" s="52">
-        <f>'NREL ATB 2022'!O154/'NREL ATB 2022'!N154-1</f>
-        <v>7.3346874492989933E-3</v>
-      </c>
-      <c r="L15" s="52">
-        <f>'NREL ATB 2022'!P154/'NREL ATB 2022'!O154-1</f>
-        <v>7.1490768505353408E-3</v>
-      </c>
-      <c r="M15" s="52">
-        <f>'NREL ATB 2022'!Q154/'NREL ATB 2022'!P154-1</f>
-        <v>3.2594762526094723E-3</v>
-      </c>
-      <c r="N15" s="52">
-        <f>'NREL ATB 2022'!R154/'NREL ATB 2022'!Q154-1</f>
-        <v>3.1528483620695269E-3</v>
-      </c>
-      <c r="O15" s="52">
-        <f>'NREL ATB 2022'!S154/'NREL ATB 2022'!R154-1</f>
-        <v>3.0595696533102235E-3</v>
-      </c>
-      <c r="P15" s="52">
-        <f>'NREL ATB 2022'!T154/'NREL ATB 2022'!S154-1</f>
-        <v>2.977206493658402E-3</v>
-      </c>
-      <c r="Q15" s="52">
-        <f>'NREL ATB 2022'!U154/'NREL ATB 2022'!T154-1</f>
-        <v>2.9038839066541922E-3</v>
-      </c>
-      <c r="R15" s="52">
-        <f>'NREL ATB 2022'!V154/'NREL ATB 2022'!U154-1</f>
-        <v>2.8381339214920143E-3</v>
-      </c>
-      <c r="S15" s="52">
-        <f>'NREL ATB 2022'!W154/'NREL ATB 2022'!V154-1</f>
-        <v>2.7787907843330739E-3</v>
-      </c>
-      <c r="T15" s="52">
-        <f>'NREL ATB 2022'!X154/'NREL ATB 2022'!W154-1</f>
-        <v>2.7249169631895498E-3</v>
-      </c>
-      <c r="U15" s="52">
-        <f>'NREL ATB 2022'!Y154/'NREL ATB 2022'!X154-1</f>
-        <v>2.6757498811897928E-3</v>
-      </c>
-      <c r="V15" s="52">
-        <f>'NREL ATB 2022'!Z154/'NREL ATB 2022'!Y154-1</f>
-        <v>2.6306629054659858E-3</v>
-      </c>
-      <c r="W15" s="52">
-        <f>'NREL ATB 2022'!AA154/'NREL ATB 2022'!Z154-1</f>
-        <v>2.5891363303196524E-3</v>
-      </c>
-      <c r="X15" s="52">
-        <f>'NREL ATB 2022'!AB154/'NREL ATB 2022'!AA154-1</f>
-        <v>2.5507354896165957E-3</v>
-      </c>
-      <c r="Y15" s="52">
-        <f>'NREL ATB 2022'!AC154/'NREL ATB 2022'!AB154-1</f>
-        <v>2.5150940350919804E-3</v>
-      </c>
-      <c r="Z15" s="52">
-        <f>'NREL ATB 2022'!AD154/'NREL ATB 2022'!AC154-1</f>
-        <v>2.4819010118353191E-3</v>
-      </c>
-      <c r="AA15" s="52">
-        <f>'NREL ATB 2022'!AE154/'NREL ATB 2022'!AD154-1</f>
-        <v>2.4508907615565789E-3</v>
-      </c>
-      <c r="AB15" s="52">
-        <f>'NREL ATB 2022'!AF154/'NREL ATB 2022'!AE154-1</f>
-        <v>2.4218349571687448E-3</v>
-      </c>
-      <c r="AC15" s="52">
-        <f>'NREL ATB 2022'!AG154/'NREL ATB 2022'!AF154-1</f>
-        <v>2.3945362615727106E-3</v>
-      </c>
-      <c r="AD15" s="52">
-        <f>'NREL ATB 2022'!AH154/'NREL ATB 2022'!AG154-1</f>
-        <v>2.3688232369343254E-3</v>
-      </c>
-      <c r="AE15" s="52">
-        <f>'NREL ATB 2022'!AI154/'NREL ATB 2022'!AH154-1</f>
-        <v>2.344546225858668E-3</v>
-      </c>
-      <c r="AF15" s="52">
-        <f>'NREL ATB 2022'!AJ154/'NREL ATB 2022'!AI154-1</f>
-        <v>2.3215739946480518E-3</v>
+      <c r="D15" s="55">
+        <f>'NREL ATB 2022'!H154/'NREL ATB 2022'!$F154-1</f>
+        <v>2.2699435310093774E-2</v>
+      </c>
+      <c r="E15" s="55">
+        <f>'NREL ATB 2022'!I154/'NREL ATB 2022'!$F154-1</f>
+        <v>3.2546880015423607E-2</v>
+      </c>
+      <c r="F15" s="55">
+        <f>'NREL ATB 2022'!J154/'NREL ATB 2022'!$F154-1</f>
+        <v>4.1815317746726643E-2</v>
+      </c>
+      <c r="G15" s="55">
+        <f>'NREL ATB 2022'!K154/'NREL ATB 2022'!$F154-1</f>
+        <v>5.0659959260966447E-2</v>
+      </c>
+      <c r="H15" s="55">
+        <f>'NREL ATB 2022'!L154/'NREL ATB 2022'!$F154-1</f>
+        <v>5.9180918678805927E-2</v>
+      </c>
+      <c r="I15" s="55">
+        <f>'NREL ATB 2022'!M154/'NREL ATB 2022'!$F154-1</f>
+        <v>6.7446553219019378E-2</v>
+      </c>
+      <c r="J15" s="55">
+        <f>'NREL ATB 2022'!N154/'NREL ATB 2022'!$F154-1</f>
+        <v>7.5505619303541049E-2</v>
+      </c>
+      <c r="K15" s="55">
+        <f>'NREL ATB 2022'!O154/'NREL ATB 2022'!$F154-1</f>
+        <v>8.3394116871097212E-2</v>
+      </c>
+      <c r="L15" s="55">
+        <f>'NREL ATB 2022'!P154/'NREL ATB 2022'!$F154-1</f>
+        <v>9.1139384672026535E-2</v>
+      </c>
+      <c r="M15" s="55">
+        <f>'NREL ATB 2022'!Q154/'NREL ATB 2022'!$F154-1</f>
+        <v>9.4695927584651951E-2</v>
+      </c>
+      <c r="N15" s="55">
+        <f>'NREL ATB 2022'!R154/'NREL ATB 2022'!$F154-1</f>
+        <v>9.8147337846901328E-2</v>
+      </c>
+      <c r="O15" s="55">
+        <f>'NREL ATB 2022'!S154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.10150719611664116</v>
+      </c>
+      <c r="P15" s="55">
+        <f>'NREL ATB 2022'!T154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.10478661049373117</v>
+      </c>
+      <c r="Q15" s="55">
+        <f>'NREL ATB 2022'!U154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.10799478255223094</v>
+      </c>
+      <c r="R15" s="55">
+        <f>'NREL ATB 2022'!V154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.11113942012942868</v>
+      </c>
+      <c r="S15" s="55">
+        <f>'NREL ATB 2022'!W154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.11422704411019358</v>
+      </c>
+      <c r="T15" s="55">
+        <f>'NREL ATB 2022'!X154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.11726322028353398</v>
+      </c>
+      <c r="U15" s="55">
+        <f>'NREL ATB 2022'!Y154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.12025273721246532</v>
+      </c>
+      <c r="V15" s="55">
+        <f>'NREL ATB 2022'!Z154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.12319974453299687</v>
+      </c>
+      <c r="W15" s="55">
+        <f>'NREL ATB 2022'!AA154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.12610786179777289</v>
+      </c>
+      <c r="X15" s="55">
+        <f>'NREL ATB 2022'!AB154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.1289802650859968</v>
+      </c>
+      <c r="Y15" s="55">
+        <f>'NREL ATB 2022'!AC154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.13181975661645118</v>
+      </c>
+      <c r="Z15" s="55">
+        <f>'NREL ATB 2022'!AD154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.13462882121561259</v>
+      </c>
+      <c r="AA15" s="55">
+        <f>'NREL ATB 2022'!AE154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.13740967251132563</v>
+      </c>
+      <c r="AB15" s="55">
+        <f>'NREL ATB 2022'!AF154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.1401642910168357</v>
+      </c>
+      <c r="AC15" s="55">
+        <f>'NREL ATB 2022'!AG154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.14289445575582582</v>
+      </c>
+      <c r="AD15" s="55">
+        <f>'NREL ATB 2022'!AH154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.1456017706999837</v>
+      </c>
+      <c r="AE15" s="55">
+        <f>'NREL ATB 2022'!AI154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.14828768700781536</v>
+      </c>
+      <c r="AF15" s="55">
+        <f>'NREL ATB 2022'!AJ154/'NREL ATB 2022'!$F154-1</f>
+        <v>0.15095352184034727</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -16769,7 +16763,7 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -16867,7 +16861,7 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18">
         <v>0</v>

</xml_diff>